<commit_message>
updating proposal list for the final subset and fixing hyperlinks
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_FINAL.xlsx
+++ b/app/data/wto_proposal_settings_master_FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B85E2BC-028E-374A-ABD8-F6BD376CFBFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D9A2B-5854-5541-8320-F623DAD35AB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="1140" windowWidth="34160" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="464">
   <si>
     <t>proposal</t>
   </si>
@@ -1393,12 +1393,6 @@
     <t>NOVEMBER Chair's text - higher impact version (only managed get sustainability exemption for domestic, but all subisdies to high seas fishing are prohibited high seas fishing)</t>
   </si>
   <si>
-    <t>NOVEMBER Chair's text - sustainability criteria (no 20% assumption)</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;We assume that final determinations are made by existing RFMO/A vessel lists, and by flag and coastal Member states.&lt;/li&gt;&lt;li&gt;No publicly available data exist for most flag and subsidizing Members, nor for coastal Members. The possible effects of modeling this proposal is therefore a conservative interpretation of this text. Users are free to explore a more ambitious interpretation by making their own assumptions about the expected IUU-findings.&lt;/li&gt;&lt;li&gt;No proportionality or the duration of prohibition is considered.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>Chair's text - Nov 2021 [Managed exemption for domestic only]</t>
   </si>
   <si>
@@ -1409,12 +1403,6 @@
   </si>
   <si>
     <t>WT/MIN(21)/W/5 | Managed exemption for domestic only</t>
-  </si>
-  <si>
-    <t>WT/MIN(21)/W/5 | Sustainability scenario + No expected IUU finding</t>
-  </si>
-  <si>
-    <t>Chair's text - Nov 2021 [Sustainability scenario + No expected IUU finding]</t>
   </si>
   <si>
     <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. It is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could only be acquired by vessels fulfilling our management criteria. We note that this may still be a conservative interpretation of this text because our management criteria are determined based on the location in which the fishing takes place, as opposed to by the flag- or subsidizing Member state.&lt;/li&gt;&lt;li&gt;This text would also prohibit subsidies to fishing in areas beyond the subsidizing Member's national jurisdiction.&lt;/li&gt;&lt;li&gt;As written, such a prohibition may not apply if a Member could satistfy the same sustainability criteria, unless the fishing activity falls outside the jurisdiction of a RFMO/A. Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale whether vessels are fishing for species governed by those RFMO/As at any given point in time. We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas or in the EEZs of other coastal states to be prohibited. We note that this may be an amibitious interpretation of the prohibition on subsidies to fishing in areas beyond national jurisdictions.&lt;/li&gt;&lt;/ol&gt;</t>
@@ -2384,11 +2372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CV52"/>
+  <dimension ref="A1:CV51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4431,7 +4419,7 @@
     </row>
     <row r="24" spans="1:100" ht="182" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>62</v>
@@ -7799,13 +7787,13 @@
         <v>328</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F49" s="9">
         <v>44524</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>39</v>
@@ -7832,7 +7820,7 @@
         <v>331</v>
       </c>
       <c r="P49" s="20" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="Q49" s="20" t="s">
         <v>454</v>
@@ -7942,13 +7930,13 @@
         <v>328</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F50" s="9">
         <v>44524</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>39</v>
@@ -7975,7 +7963,7 @@
         <v>331</v>
       </c>
       <c r="P50" s="20" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Q50" s="20" t="s">
         <v>454</v>
@@ -8071,66 +8059,27 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:100" ht="297" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:100" ht="42" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="F51" s="9">
-        <v>44524</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="H51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="G51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H51" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I51" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="L51" s="20" t="s">
-        <v>458</v>
-      </c>
-      <c r="M51" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="N51" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="O51" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="P51" s="20" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q51" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="R51" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="S51" s="8" t="s">
-        <v>282</v>
-      </c>
       <c r="T51" s="8" t="s">
         <v>150</v>
+      </c>
+      <c r="U51" s="8">
+        <v>20</v>
       </c>
       <c r="V51" s="8" t="s">
         <v>149</v>
@@ -8141,270 +8090,181 @@
       <c r="Z51" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="AB51" s="8">
+        <v>5</v>
+      </c>
       <c r="AC51" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="AE51" s="8">
+        <v>5</v>
+      </c>
       <c r="AF51" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="AI51" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="AJ51" s="8" t="s">
-        <v>181</v>
+      <c r="AH51" s="8">
+        <v>5</v>
       </c>
       <c r="AK51" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="AM51" s="8">
+        <v>5</v>
+      </c>
+      <c r="AN51" s="8">
+        <v>24</v>
+      </c>
+      <c r="AO51" s="8">
+        <v>100</v>
+      </c>
+      <c r="AP51" s="8">
+        <v>400</v>
+      </c>
       <c r="AQ51" s="8" t="s">
         <v>150</v>
       </c>
       <c r="AR51" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="AT51" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU51" s="8">
+        <v>5</v>
+      </c>
       <c r="AV51" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="AX51" s="8">
+        <v>5</v>
+      </c>
+      <c r="AY51" s="8">
+        <v>5</v>
+      </c>
       <c r="AZ51" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="BD51" s="8" t="s">
-        <v>190</v>
+      <c r="BB51" s="8">
+        <v>5</v>
+      </c>
+      <c r="BC51" s="8">
+        <v>5</v>
       </c>
       <c r="BE51" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="BF51" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="BH51" s="8">
+        <v>5</v>
+      </c>
+      <c r="BI51" s="8">
+        <v>24</v>
+      </c>
+      <c r="BJ51" s="8">
+        <v>100</v>
+      </c>
+      <c r="BK51" s="8">
+        <v>400</v>
+      </c>
       <c r="BL51" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="BM51" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="BN51" s="8" t="s">
-        <v>188</v>
+        <v>150</v>
+      </c>
+      <c r="BO51" s="8">
+        <v>5</v>
+      </c>
+      <c r="BP51" s="8">
+        <v>5</v>
       </c>
       <c r="BQ51" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="BR51" s="8" t="s">
-        <v>188</v>
+        <v>150</v>
+      </c>
+      <c r="BS51" s="8">
+        <v>5</v>
+      </c>
+      <c r="BT51" s="8">
+        <v>5</v>
       </c>
       <c r="BU51" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="BW51" s="8">
+        <v>5</v>
+      </c>
+      <c r="BX51" s="8">
+        <v>5</v>
+      </c>
       <c r="BY51" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:100" ht="42" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="G52" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="U52" s="8">
-        <v>20</v>
-      </c>
-      <c r="V52" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB52" s="8">
+      <c r="BZ51" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="CA51" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="CB51" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="CC51" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="CD51" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="CE51" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="CF51" s="8">
+        <v>50</v>
+      </c>
+      <c r="CG51" s="14">
         <v>5</v>
       </c>
-      <c r="AC52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE52" s="8">
+      <c r="CH51" s="14">
         <v>5</v>
       </c>
-      <c r="AF52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH52" s="8">
+      <c r="CI51" s="14">
         <v>5</v>
       </c>
-      <c r="AK52" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AM52" s="8">
+      <c r="CJ51" s="14">
         <v>5</v>
       </c>
-      <c r="AN52" s="8">
-        <v>24</v>
-      </c>
-      <c r="AO52" s="8">
-        <v>100</v>
-      </c>
-      <c r="AP52" s="8">
-        <v>400</v>
-      </c>
-      <c r="AQ52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AR52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT52" s="8">
+      <c r="CK51" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="CL51" s="8">
         <v>5</v>
       </c>
-      <c r="AU52" s="8">
+      <c r="CM51" s="8">
         <v>5</v>
       </c>
-      <c r="AV52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AX52" s="8">
+      <c r="CN51" s="14">
         <v>5</v>
       </c>
-      <c r="AY52" s="8">
+      <c r="CO51" s="14">
         <v>5</v>
       </c>
-      <c r="AZ52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BB52" s="8">
+      <c r="CP51" s="14">
         <v>5</v>
       </c>
-      <c r="BC52" s="8">
+      <c r="CQ51" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="CR51" s="8">
         <v>5</v>
       </c>
-      <c r="BE52" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BH52" s="8">
+      <c r="CS51" s="8">
         <v>5</v>
       </c>
-      <c r="BI52" s="8">
-        <v>24</v>
-      </c>
-      <c r="BJ52" s="8">
-        <v>100</v>
-      </c>
-      <c r="BK52" s="8">
-        <v>400</v>
-      </c>
-      <c r="BL52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BM52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BO52" s="8">
+      <c r="CT51" s="14">
         <v>5</v>
       </c>
-      <c r="BP52" s="8">
+      <c r="CU51" s="14">
         <v>5</v>
       </c>
-      <c r="BQ52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BS52" s="8">
-        <v>5</v>
-      </c>
-      <c r="BT52" s="8">
-        <v>5</v>
-      </c>
-      <c r="BU52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BW52" s="8">
-        <v>5</v>
-      </c>
-      <c r="BX52" s="8">
-        <v>5</v>
-      </c>
-      <c r="BY52" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BZ52" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="CA52" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="CB52" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="CC52" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="CD52" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="CE52" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="CF52" s="8">
-        <v>50</v>
-      </c>
-      <c r="CG52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CH52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CI52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CJ52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CK52" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="CL52" s="8">
-        <v>5</v>
-      </c>
-      <c r="CM52" s="8">
-        <v>5</v>
-      </c>
-      <c r="CN52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CO52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CP52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CQ52" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="CR52" s="8">
-        <v>5</v>
-      </c>
-      <c r="CS52" s="8">
-        <v>5</v>
-      </c>
-      <c r="CT52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CU52" s="14">
-        <v>5</v>
-      </c>
-      <c r="CV52" s="14">
+      <c r="CV51" s="14">
         <v>5</v>
       </c>
     </row>

</xml_diff>